<commit_message>
new downloaders and parsers to scrap the ACM website
</commit_message>
<xml_diff>
--- a/CHI-stats.xlsx
+++ b/CHI-stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="0" windowWidth="30820" windowHeight="19400" tabRatio="725" activeTab="1"/>
+    <workbookView xWindow="660" yWindow="0" windowWidth="30820" windowHeight="19400" tabRatio="725" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="ACM" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="519">
   <si>
     <t xml:space="preserve">Year </t>
   </si>
@@ -1500,6 +1500,99 @@
   </si>
   <si>
     <t>ITS / Tabletop</t>
+  </si>
+  <si>
+    <t>http://dl.acm.org/citation.cfm?id=225434&amp;CFID=301718928&amp;CFTOKEN=65027953</t>
+  </si>
+  <si>
+    <t>citation.cfm?id=225434</t>
+  </si>
+  <si>
+    <t>DIS'95</t>
+  </si>
+  <si>
+    <t>DIS'97</t>
+  </si>
+  <si>
+    <t>http://dl.acm.org/citation.cfm?id=263552&amp;picked=prox&amp;CFID=301718928&amp;CFTOKEN=65027953</t>
+  </si>
+  <si>
+    <t>http://dl.acm.org/citation.cfm?id=347642&amp;picked=prox&amp;CFID=301718928&amp;CFTOKEN=65027953</t>
+  </si>
+  <si>
+    <t>citation.cfm?id=347642</t>
+  </si>
+  <si>
+    <t>citation.cfm?id=263552</t>
+  </si>
+  <si>
+    <t>DIS'00</t>
+  </si>
+  <si>
+    <t>DIS'02</t>
+  </si>
+  <si>
+    <t>DIS'04</t>
+  </si>
+  <si>
+    <t>DIS'06</t>
+  </si>
+  <si>
+    <t>DIS'08</t>
+  </si>
+  <si>
+    <t>DIS'10</t>
+  </si>
+  <si>
+    <t>DIS'12</t>
+  </si>
+  <si>
+    <t>http://dl.acm.org/citation.cfm?id=1013115&amp;picked=prox&amp;CFID=301718928&amp;CFTOKEN=65027953</t>
+  </si>
+  <si>
+    <t>citation.cfm?id=1013115</t>
+  </si>
+  <si>
+    <t>http://dl.acm.org/citation.cfm?id=778712&amp;picked=prox&amp;CFID=301718928&amp;CFTOKEN=65027953</t>
+  </si>
+  <si>
+    <t>citation.cfm?id=778712</t>
+  </si>
+  <si>
+    <t>http://dl.acm.org/citation.cfm?id=1142405&amp;picked=prox&amp;CFID=301718928&amp;CFTOKEN=65027953</t>
+  </si>
+  <si>
+    <t>citation.cfm?id=1142405</t>
+  </si>
+  <si>
+    <t>http://dl.acm.org/citation.cfm?id=1394445&amp;picked=prox&amp;CFID=301718928&amp;CFTOKEN=65027953</t>
+  </si>
+  <si>
+    <t>citation.cfm?id=1394445</t>
+  </si>
+  <si>
+    <t>http://dl.acm.org/citation.cfm?id=1858171&amp;picked=prox&amp;CFID=301718928&amp;CFTOKEN=65027953</t>
+  </si>
+  <si>
+    <t>citation.cfm?id=1858171</t>
+  </si>
+  <si>
+    <t>http://dl.acm.org/citation.cfm?id=2317956&amp;picked=prox&amp;CFID=301718928&amp;CFTOKEN=65027953</t>
+  </si>
+  <si>
+    <t>citation.cfm?id=2317956</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Page contains workshops and demos</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Keynotes?</t>
   </si>
 </sst>
 </file>
@@ -1565,9 +1658,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1695,7 +1789,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="92">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1785,6 +1879,7 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2118,7 +2213,7 @@
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3246,10 +3341,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3295,6 +3390,15 @@
       <c r="A3" t="s">
         <v>360</v>
       </c>
+      <c r="B3">
+        <v>130</v>
+      </c>
+      <c r="C3">
+        <v>45</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.35</v>
+      </c>
       <c r="G3" t="s">
         <v>350</v>
       </c>
@@ -3328,6 +3432,15 @@
       <c r="A6" t="s">
         <v>357</v>
       </c>
+      <c r="B6">
+        <v>102</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.39</v>
+      </c>
       <c r="G6" t="s">
         <v>347</v>
       </c>
@@ -3339,6 +3452,15 @@
       <c r="A7" t="s">
         <v>356</v>
       </c>
+      <c r="B7">
+        <v>99</v>
+      </c>
+      <c r="C7">
+        <v>55</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.56000000000000005</v>
+      </c>
       <c r="G7" t="s">
         <v>346</v>
       </c>
@@ -3350,6 +3472,15 @@
       <c r="A8" t="s">
         <v>355</v>
       </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>44</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.44</v>
+      </c>
       <c r="G8" t="s">
         <v>345</v>
       </c>
@@ -3361,6 +3492,15 @@
       <c r="A9" t="s">
         <v>354</v>
       </c>
+      <c r="B9">
+        <v>118</v>
+      </c>
+      <c r="C9">
+        <v>41</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.35</v>
+      </c>
       <c r="G9" t="s">
         <v>344</v>
       </c>
@@ -3372,6 +3512,15 @@
       <c r="A10" t="s">
         <v>353</v>
       </c>
+      <c r="B10">
+        <v>120</v>
+      </c>
+      <c r="C10">
+        <v>47</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.39</v>
+      </c>
       <c r="G10" t="s">
         <v>343</v>
       </c>
@@ -3383,12 +3532,24 @@
       <c r="A11" t="s">
         <v>352</v>
       </c>
+      <c r="B11">
+        <v>147</v>
+      </c>
+      <c r="C11">
+        <v>61</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.41</v>
+      </c>
       <c r="G11" t="s">
         <v>342</v>
       </c>
       <c r="N11">
         <v>2011</v>
       </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="D12" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A2:N11">
@@ -3897,7 +4058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -4519,7 +4680,7 @@
         <v>2742</v>
       </c>
       <c r="G19" s="7">
-        <f t="shared" ref="G19:G31" si="1">F19/D19</f>
+        <f t="shared" ref="G19:G30" si="1">F19/D19</f>
         <v>38.083333333333336</v>
       </c>
       <c r="H19" t="s">
@@ -5009,7 +5170,7 @@
   <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="A1:H26"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6570,11 +6731,14 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:O19"/>
+      <pane ySplit="3860" topLeftCell="A13" activePane="bottomLeft"/>
+      <selection activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="7" max="7" width="25.83203125" customWidth="1"/>
     <col min="8" max="8" width="25.33203125" customWidth="1"/>
     <col min="18" max="18" width="10.83203125" style="7"/>
   </cols>
@@ -7001,13 +7165,202 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>122</v>
+      </c>
+      <c r="O1" t="s">
+        <v>217</v>
+      </c>
+      <c r="P1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>490</v>
+      </c>
+      <c r="G2" t="s">
+        <v>489</v>
+      </c>
+      <c r="H2" t="s">
+        <v>488</v>
+      </c>
+      <c r="O2">
+        <v>1995</v>
+      </c>
+      <c r="P2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>491</v>
+      </c>
+      <c r="G3" t="s">
+        <v>495</v>
+      </c>
+      <c r="H3" t="s">
+        <v>492</v>
+      </c>
+      <c r="O3">
+        <v>1997</v>
+      </c>
+      <c r="P3" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>496</v>
+      </c>
+      <c r="G4" t="s">
+        <v>494</v>
+      </c>
+      <c r="H4" t="s">
+        <v>493</v>
+      </c>
+      <c r="O4">
+        <v>2000</v>
+      </c>
+      <c r="P4" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>497</v>
+      </c>
+      <c r="G5" t="s">
+        <v>506</v>
+      </c>
+      <c r="H5" t="s">
+        <v>505</v>
+      </c>
+      <c r="O5">
+        <v>2002</v>
+      </c>
+      <c r="P5" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>498</v>
+      </c>
+      <c r="G6" t="s">
+        <v>504</v>
+      </c>
+      <c r="H6" t="s">
+        <v>503</v>
+      </c>
+      <c r="O6">
+        <v>2004</v>
+      </c>
+      <c r="P6" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>499</v>
+      </c>
+      <c r="G7" t="s">
+        <v>508</v>
+      </c>
+      <c r="H7" t="s">
+        <v>507</v>
+      </c>
+      <c r="O7">
+        <v>2006</v>
+      </c>
+      <c r="P7" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>500</v>
+      </c>
+      <c r="G8" t="s">
+        <v>510</v>
+      </c>
+      <c r="H8" t="s">
+        <v>509</v>
+      </c>
+      <c r="O8">
+        <v>2008</v>
+      </c>
+      <c r="P8" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>501</v>
+      </c>
+      <c r="G9" t="s">
+        <v>512</v>
+      </c>
+      <c r="H9" t="s">
+        <v>511</v>
+      </c>
+      <c r="O9">
+        <v>2010</v>
+      </c>
+      <c r="P9" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>502</v>
+      </c>
+      <c r="G10" t="s">
+        <v>514</v>
+      </c>
+      <c r="H10" t="s">
+        <v>513</v>
+      </c>
+      <c r="O10">
+        <v>2012</v>
+      </c>
+      <c r="P10" t="s">
+        <v>516</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>